<commit_message>
Almost, but no cookie
Property added, but won't open in ecoEditor.
</commit_message>
<xml_diff>
--- a/waste_water_tool/documentation/WW_properties.xlsx
+++ b/waste_water_tool/documentation/WW_properties.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="Missing" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="247">
   <si>
     <t>dd13a45c-ddd8-414d-821f-dfe31c7d2868</t>
   </si>
@@ -1699,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3901,6 +3901,53 @@
       <c r="N50" s="24"/>
       <c r="O50" s="25" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>244</v>
+      </c>
+      <c r="B51" t="s">
+        <v>245</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>246</v>
+      </c>
+      <c r="E51">
+        <v>666</v>
+      </c>
+      <c r="F51">
+        <v>666</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="M51" t="s">
+        <v>79</v>
+      </c>
+      <c r="N51" t="s">
+        <v>79</v>
+      </c>
+      <c r="O51" s="29" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tests w/o news properties
Also fails now.
</commit_message>
<xml_diff>
--- a/waste_water_tool/documentation/WW_properties.xlsx
+++ b/waste_water_tool/documentation/WW_properties.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="288">
   <si>
     <t>dd13a45c-ddd8-414d-821f-dfe31c7d2868</t>
   </si>
@@ -610,12 +610,6 @@
   </si>
   <si>
     <t>Amount</t>
-  </si>
-  <si>
-    <t>MISSING__Soluble Kjeldahl SKN as N</t>
-  </si>
-  <si>
-    <t>MISSING__Total Kjeldahl TKN as N</t>
   </si>
   <si>
     <t>MISSING__Particulate P-part. as P</t>
@@ -861,30 +855,6 @@
       </rPr>
       <t>PO4 as P</t>
     </r>
-  </si>
-  <si>
-    <t>mass concentration, soluble Kjeldahl SKN as N</t>
-  </si>
-  <si>
-    <t>mass concentration, total Kjeldahl TKN as N</t>
-  </si>
-  <si>
-    <t>Mass concentration of soluble Kjeldahl SKN as N</t>
-  </si>
-  <si>
-    <t>Mass concentration of total Kjeldahl TKN as N</t>
-  </si>
-  <si>
-    <t>Mass concentration of particulate phosphorus as P</t>
-  </si>
-  <si>
-    <t>mass concentration, particulate phosphorus as P</t>
-  </si>
-  <si>
-    <t>mass concentration, total phosphorus as P</t>
-  </si>
-  <si>
-    <t>Mass concentration of total phosphorus as P</t>
   </si>
   <si>
     <t>Boron</t>
@@ -1434,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y87"/>
+  <dimension ref="A1:Y85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1466,58 +1436,58 @@
         <v>193</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>186</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -1583,10 +1553,10 @@
         <v>37</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -1652,10 +1622,10 @@
         <v>37</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -1721,10 +1691,10 @@
         <v>37</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -1790,10 +1760,10 @@
         <v>37</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -1859,13 +1829,13 @@
         <v>39</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -1931,13 +1901,13 @@
         <v>39</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2003,13 +1973,13 @@
         <v>39</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2075,13 +2045,13 @@
         <v>39</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2147,13 +2117,13 @@
         <v>39</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2219,13 +2189,13 @@
         <v>39</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2291,13 +2261,13 @@
         <v>40</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2363,13 +2333,13 @@
         <v>38</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2435,13 +2405,13 @@
         <v>38</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2507,13 +2477,13 @@
         <v>38</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="V15" s="5" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
@@ -2582,7 +2552,7 @@
         <v>42</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
@@ -2653,7 +2623,7 @@
         <v>43</v>
       </c>
       <c r="V17" s="5" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
@@ -2724,7 +2694,7 @@
         <v>44</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
@@ -2795,10 +2765,10 @@
         <v>45</v>
       </c>
       <c r="V19" s="5" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W19" s="5" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
@@ -2869,10 +2839,10 @@
         <v>46</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
@@ -2943,7 +2913,7 @@
         <v>47</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
@@ -3014,7 +2984,7 @@
         <v>48</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
@@ -3085,7 +3055,7 @@
         <v>49</v>
       </c>
       <c r="V23" s="5" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
@@ -3156,7 +3126,7 @@
         <v>50</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
@@ -3227,7 +3197,7 @@
         <v>51</v>
       </c>
       <c r="V25" s="5" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
@@ -3298,10 +3268,10 @@
         <v>52</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="W26" s="5" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="X26" s="5"/>
     </row>
@@ -3371,7 +3341,7 @@
         <v>53</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
@@ -3442,7 +3412,7 @@
         <v>54</v>
       </c>
       <c r="V28" s="5" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
@@ -3513,7 +3483,7 @@
         <v>55</v>
       </c>
       <c r="V29" s="5" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
@@ -3584,7 +3554,7 @@
         <v>56</v>
       </c>
       <c r="V30" s="5" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
@@ -3655,7 +3625,7 @@
         <v>57</v>
       </c>
       <c r="V31" s="5" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
@@ -3726,7 +3696,7 @@
         <v>58</v>
       </c>
       <c r="V32" s="5" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
@@ -3797,7 +3767,7 @@
         <v>59</v>
       </c>
       <c r="V33" s="5" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
@@ -3868,7 +3838,7 @@
         <v>60</v>
       </c>
       <c r="V34" s="5" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="W34" s="5"/>
       <c r="X34" s="5"/>
@@ -3939,7 +3909,7 @@
         <v>61</v>
       </c>
       <c r="V35" s="5" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="W35" s="5"/>
       <c r="X35" s="5"/>
@@ -4010,7 +3980,7 @@
         <v>62</v>
       </c>
       <c r="V36" s="5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="W36" s="5"/>
       <c r="X36" s="5"/>
@@ -4081,7 +4051,7 @@
         <v>63</v>
       </c>
       <c r="V37" s="5" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
@@ -4152,7 +4122,7 @@
         <v>64</v>
       </c>
       <c r="V38" s="5" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="W38" s="5"/>
       <c r="X38" s="5"/>
@@ -4223,7 +4193,7 @@
         <v>65</v>
       </c>
       <c r="V39" s="5" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="W39" s="5"/>
       <c r="X39" s="5"/>
@@ -4294,7 +4264,7 @@
         <v>66</v>
       </c>
       <c r="V40" s="5" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
@@ -4365,7 +4335,7 @@
         <v>67</v>
       </c>
       <c r="V41" s="5" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
@@ -4436,7 +4406,7 @@
         <v>68</v>
       </c>
       <c r="V42" s="5" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
@@ -4507,7 +4477,7 @@
         <v>69</v>
       </c>
       <c r="V43" s="5" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="W43" s="5"/>
       <c r="X43" s="5"/>
@@ -4578,7 +4548,7 @@
         <v>70</v>
       </c>
       <c r="V44" s="5" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="W44" s="5"/>
       <c r="X44" s="5"/>
@@ -4649,7 +4619,7 @@
         <v>71</v>
       </c>
       <c r="V45" s="5" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="W45" s="5"/>
       <c r="X45" s="5"/>
@@ -4720,7 +4690,7 @@
         <v>72</v>
       </c>
       <c r="V46" s="5" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="W46" s="5"/>
       <c r="X46" s="5"/>
@@ -4791,7 +4761,7 @@
         <v>73</v>
       </c>
       <c r="V47" s="5" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="W47" s="5"/>
       <c r="X47" s="5"/>
@@ -4862,7 +4832,7 @@
         <v>74</v>
       </c>
       <c r="V48" s="5" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="W48" s="5"/>
       <c r="X48" s="5"/>
@@ -4933,7 +4903,7 @@
         <v>75</v>
       </c>
       <c r="V49" s="5" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="W49" s="5"/>
       <c r="X49" s="5"/>
@@ -5004,309 +4974,175 @@
         <v>76</v>
       </c>
       <c r="V50" s="5" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="W50" s="5"/>
       <c r="X50" s="5"/>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>196</v>
+        <v>278</v>
       </c>
       <c r="B51" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="E51">
-        <v>0.72191434380727115</v>
+        <v>7.4950531145233534E-2</v>
       </c>
       <c r="F51">
-        <v>4.3980042977783476E-3</v>
+        <v>4.4797382932572115E-3</v>
       </c>
       <c r="G51">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I51">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L51">
-        <v>0.94908627586015371</v>
+        <v>0.71396399307893577</v>
       </c>
       <c r="M51">
-        <v>4.7077124962892148E-3</v>
+        <v>4.9997455849664111E-3</v>
       </c>
       <c r="N51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S51">
         <f>1-L51</f>
-        <v>5.0913724139846295E-2</v>
+        <v>0.28603600692106423</v>
       </c>
       <c r="T51" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U51" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="V51" s="5" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="W51" s="4" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>197</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>295</v>
+        <v>281</v>
+      </c>
+      <c r="B52" t="s">
+        <v>282</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="E52">
-        <v>3.3187972617449324E-2</v>
+        <v>0.26473887088891568</v>
       </c>
       <c r="F52">
-        <v>6.7249171695745701E-3</v>
+        <v>7.4975960537261967E-3</v>
       </c>
       <c r="G52">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>3</v>
       </c>
       <c r="I52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L52">
-        <v>0.63264015492889036</v>
+        <v>0.74951244436610531</v>
       </c>
       <c r="M52">
-        <v>2.2120885677457936E-3</v>
+        <v>2.3208881026338247E-3</v>
       </c>
       <c r="N52">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q52">
         <v>3</v>
       </c>
       <c r="R52">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S52">
         <f>1-L52</f>
-        <v>0.36735984507110964</v>
+        <v>0.25048755563389469</v>
       </c>
       <c r="T52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U52" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="V52" s="5" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="W52" s="4" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" t="s">
-        <v>288</v>
-      </c>
-      <c r="B53" t="s">
-        <v>289</v>
-      </c>
-      <c r="C53" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>290</v>
-      </c>
-      <c r="E53">
-        <v>7.4950531145233534E-2</v>
-      </c>
-      <c r="F53">
-        <v>4.4797382932572115E-3</v>
-      </c>
-      <c r="G53">
-        <v>4</v>
-      </c>
-      <c r="H53">
-        <v>4</v>
-      </c>
-      <c r="I53">
-        <v>2</v>
-      </c>
-      <c r="J53">
-        <v>1</v>
-      </c>
-      <c r="K53">
-        <v>1</v>
-      </c>
-      <c r="L53">
-        <v>0.71396399307893577</v>
-      </c>
-      <c r="M53">
-        <v>4.9997455849664111E-3</v>
-      </c>
-      <c r="N53">
-        <v>5</v>
-      </c>
-      <c r="O53">
-        <v>2</v>
-      </c>
-      <c r="P53">
-        <v>1</v>
-      </c>
-      <c r="Q53">
-        <v>5</v>
-      </c>
-      <c r="R53">
-        <v>1</v>
-      </c>
-      <c r="S53">
-        <f>1-L53</f>
-        <v>0.28603600692106423</v>
-      </c>
-      <c r="T53" t="s">
-        <v>40</v>
-      </c>
-      <c r="U53" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="V53" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="W53" s="4" t="s">
-        <v>284</v>
-      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" t="s">
-        <v>291</v>
-      </c>
-      <c r="B54" t="s">
-        <v>292</v>
-      </c>
-      <c r="C54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" t="s">
-        <v>293</v>
-      </c>
-      <c r="E54">
-        <v>0.26473887088891568</v>
-      </c>
-      <c r="F54">
-        <v>7.4975960537261967E-3</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-      <c r="H54">
-        <v>3</v>
-      </c>
-      <c r="I54">
-        <v>3</v>
-      </c>
-      <c r="J54">
-        <v>1</v>
-      </c>
-      <c r="K54">
-        <v>1</v>
-      </c>
-      <c r="L54">
-        <v>0.74951244436610531</v>
-      </c>
-      <c r="M54">
-        <v>2.3208881026338247E-3</v>
-      </c>
-      <c r="N54">
-        <v>1</v>
-      </c>
-      <c r="O54">
-        <v>3</v>
-      </c>
-      <c r="P54">
-        <v>1</v>
-      </c>
-      <c r="Q54">
-        <v>3</v>
-      </c>
-      <c r="R54">
-        <v>5</v>
-      </c>
-      <c r="S54">
-        <f>1-L54</f>
-        <v>0.25048755563389469</v>
-      </c>
-      <c r="T54" t="s">
-        <v>40</v>
-      </c>
-      <c r="U54" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="V54" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="W54" s="4" t="s">
-        <v>284</v>
-      </c>
+      <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="C58" s="5"/>
@@ -5327,6 +5163,7 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="C62" s="5"/>
@@ -5337,7 +5174,6 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" s="5"/>
@@ -5448,16 +5284,6 @@
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="5"/>
-    </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:U1">
@@ -5472,10 +5298,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A2:W3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:W4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5483,292 +5309,148 @@
     <col min="3" max="3" width="43.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E1">
-        <v>0.72191434380727115</v>
-      </c>
-      <c r="F1">
-        <v>4.3980042977783476E-3</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>2</v>
-      </c>
-      <c r="I1">
-        <v>5</v>
-      </c>
-      <c r="J1">
-        <v>4</v>
-      </c>
-      <c r="K1">
-        <v>4</v>
-      </c>
-      <c r="L1">
-        <v>0.94908627586015371</v>
-      </c>
-      <c r="M1">
-        <v>4.7077124962892148E-3</v>
-      </c>
-      <c r="N1">
-        <v>3</v>
-      </c>
-      <c r="O1">
-        <v>4</v>
-      </c>
-      <c r="P1">
-        <v>4</v>
-      </c>
-      <c r="Q1">
-        <v>3</v>
-      </c>
-      <c r="R1">
-        <v>4</v>
-      </c>
-      <c r="S1">
-        <f>1-L1</f>
-        <v>5.0913724139846295E-2</v>
-      </c>
-      <c r="T1" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>284</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>234</v>
+        <v>286</v>
       </c>
       <c r="E2">
-        <v>3.3187972617449324E-2</v>
+        <v>0.72191434380727115</v>
       </c>
       <c r="F2">
-        <v>6.7249171695745701E-3</v>
+        <v>4.3980042977783476E-3</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L2">
-        <v>0.63264015492889036</v>
+        <v>0.94908627586015371</v>
       </c>
       <c r="M2">
-        <v>2.2120885677457936E-3</v>
+        <v>4.7077124962892148E-3</v>
       </c>
       <c r="N2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O2">
         <v>4</v>
       </c>
       <c r="P2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q2">
         <v>3</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S2">
         <f>1-L2</f>
-        <v>0.36735984507110964</v>
+        <v>5.0913724139846295E-2</v>
       </c>
       <c r="T2" t="s">
         <v>39</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" t="s">
-        <v>236</v>
+        <v>195</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>235</v>
+        <v>287</v>
       </c>
       <c r="E3">
-        <v>7.4950531145233534E-2</v>
+        <v>3.3187972617449324E-2</v>
       </c>
       <c r="F3">
-        <v>4.4797382932572115E-3</v>
+        <v>6.7249171695745701E-3</v>
       </c>
       <c r="G3">
         <v>4</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3">
-        <v>0.71396399307893577</v>
+        <v>0.63264015492889036</v>
       </c>
       <c r="M3">
-        <v>4.9997455849664111E-3</v>
+        <v>2.2120885677457936E-3</v>
       </c>
       <c r="N3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3">
         <f>1-L3</f>
-        <v>0.28603600692106423</v>
+        <v>0.36735984507110964</v>
       </c>
       <c r="T3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>238</v>
-      </c>
-      <c r="E4">
-        <v>0.26473887088891568</v>
-      </c>
-      <c r="F4">
-        <v>7.4975960537261967E-3</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0.74951244436610531</v>
-      </c>
-      <c r="M4">
-        <v>2.3208881026338247E-3</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>3</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>3</v>
-      </c>
-      <c r="R4">
-        <v>5</v>
-      </c>
-      <c r="S4">
-        <f>1-L4</f>
-        <v>0.25048755563389469</v>
-      </c>
-      <c r="T4" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the generation of user MD
</commit_message>
<xml_diff>
--- a/waste_water_tool/documentation/WW_properties.xlsx
+++ b/waste_water_tool/documentation/WW_properties.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mypy\code\wastewater_treatment_tool\waste_water_tool\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python\wastewater_treatment_tool\waste_water_tool\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8811" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WW_props" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WW_props!$A$1:$U$1</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterate="1"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="288">
   <si>
     <t>dd13a45c-ddd8-414d-821f-dfe31c7d2868</t>
   </si>
@@ -1037,7 +1037,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1403,23 +1403,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="4" max="4" width="55.89453125" customWidth="1"/>
-    <col min="10" max="11" width="19.41796875" customWidth="1"/>
-    <col min="20" max="20" width="10.26171875" customWidth="1"/>
-    <col min="21" max="21" width="35.9453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.921875" customWidth="1"/>
+    <col min="10" max="11" width="19.3828125" customWidth="1"/>
+    <col min="20" max="20" width="10.23046875" customWidth="1"/>
+    <col min="21" max="21" width="35.921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>182</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -2628,7 +2628,7 @@
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -2699,7 +2699,7 @@
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>95</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -2989,7 +2989,7 @@
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>187</v>
       </c>
@@ -3060,7 +3060,7 @@
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -3131,7 +3131,7 @@
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>107</v>
       </c>
@@ -3202,7 +3202,7 @@
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="X26" s="5"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -3346,7 +3346,7 @@
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>116</v>
       </c>
@@ -3417,7 +3417,7 @@
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>190</v>
       </c>
@@ -3488,7 +3488,7 @@
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -3630,7 +3630,7 @@
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -3701,7 +3701,7 @@
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -3772,7 +3772,7 @@
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>131</v>
       </c>
@@ -3843,7 +3843,7 @@
       <c r="W34" s="5"/>
       <c r="X34" s="5"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -3914,7 +3914,7 @@
       <c r="W35" s="5"/>
       <c r="X35" s="5"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -3985,7 +3985,7 @@
       <c r="W36" s="5"/>
       <c r="X36" s="5"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -4056,7 +4056,7 @@
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -4127,7 +4127,7 @@
       <c r="W38" s="5"/>
       <c r="X38" s="5"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -4198,7 +4198,7 @@
       <c r="W39" s="5"/>
       <c r="X39" s="5"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -4269,7 +4269,7 @@
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>152</v>
       </c>
@@ -4340,7 +4340,7 @@
       <c r="W41" s="5"/>
       <c r="X41" s="5"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -4411,7 +4411,7 @@
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -4482,7 +4482,7 @@
       <c r="W43" s="5"/>
       <c r="X43" s="5"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>161</v>
       </c>
@@ -4553,7 +4553,7 @@
       <c r="W44" s="5"/>
       <c r="X44" s="5"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -4624,7 +4624,7 @@
       <c r="W45" s="5"/>
       <c r="X45" s="5"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -4695,7 +4695,7 @@
       <c r="W46" s="5"/>
       <c r="X46" s="5"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -4766,7 +4766,7 @@
       <c r="W47" s="5"/>
       <c r="X47" s="5"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -4837,7 +4837,7 @@
       <c r="W48" s="5"/>
       <c r="X48" s="5"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>176</v>
       </c>
@@ -4908,7 +4908,7 @@
       <c r="W49" s="5"/>
       <c r="X49" s="5"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -4979,7 +4979,7 @@
       <c r="W50" s="5"/>
       <c r="X50" s="5"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>278</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>281</v>
       </c>
@@ -5123,170 +5123,306 @@
         <v>274</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C54" s="5"/>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" t="s">
+        <v>284</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>286</v>
+      </c>
+      <c r="E53">
+        <v>0.72191434380727115</v>
+      </c>
+      <c r="F53">
+        <v>4.3980042977783476E-3</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>5</v>
+      </c>
+      <c r="J53">
+        <v>4</v>
+      </c>
+      <c r="K53">
+        <v>4</v>
+      </c>
+      <c r="L53">
+        <v>0.94908627586015371</v>
+      </c>
+      <c r="M53">
+        <v>4.7077124962892148E-3</v>
+      </c>
+      <c r="N53">
+        <v>3</v>
+      </c>
+      <c r="O53">
+        <v>4</v>
+      </c>
+      <c r="P53">
+        <v>4</v>
+      </c>
+      <c r="Q53">
+        <v>3</v>
+      </c>
+      <c r="R53">
+        <v>4</v>
+      </c>
+      <c r="S53">
+        <f>1-L53</f>
+        <v>5.0913724139846295E-2</v>
+      </c>
+      <c r="T53" t="s">
+        <v>39</v>
+      </c>
+      <c r="U53" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="V53" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="W53" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>287</v>
+      </c>
+      <c r="E54">
+        <v>3.3187972617449324E-2</v>
+      </c>
+      <c r="F54">
+        <v>6.7249171695745701E-3</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <v>3</v>
+      </c>
+      <c r="I54">
+        <v>4</v>
+      </c>
+      <c r="J54">
+        <v>2</v>
+      </c>
+      <c r="K54">
+        <v>2</v>
+      </c>
+      <c r="L54">
+        <v>0.63264015492889036</v>
+      </c>
+      <c r="M54">
+        <v>2.2120885677457936E-3</v>
+      </c>
+      <c r="N54">
+        <v>4</v>
+      </c>
+      <c r="O54">
+        <v>4</v>
+      </c>
+      <c r="P54">
+        <v>3</v>
+      </c>
+      <c r="Q54">
+        <v>3</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <f>1-L54</f>
+        <v>0.36735984507110964</v>
+      </c>
+      <c r="T54" t="s">
+        <v>39</v>
+      </c>
+      <c r="U54" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="V54" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="W54" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.4">
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
     </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
     </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
     </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
     </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
     </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
     </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
     </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
     </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
     </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
     </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
     </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U1">
+  <autoFilter ref="A1:U1" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:U54">
       <sortCondition ref="T1"/>
     </sortState>
@@ -5297,19 +5433,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:XFD4"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="43.734375" customWidth="1"/>
+    <col min="3" max="3" width="43.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -5381,7 +5517,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>195</v>
       </c>

</xml_diff>